<commit_message>
add topercent && 统一为电脑pad && add 自动换行
</commit_message>
<xml_diff>
--- a/py/forWork/doc/dict.xlsx
+++ b/py/forWork/doc/dict.xlsx
@@ -65,7 +65,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z84"/>
+  <dimension ref="A1:Z110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,7 +485,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>没有使用事件</t>
         </is>
       </c>
       <c r="D2" s="2" t="n"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D3" s="2" t="n"/>
@@ -557,11 +557,11 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环内缺少内容</t>
         </is>
       </c>
       <c r="D4" s="2" t="n"/>
@@ -595,11 +595,11 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D5" s="2" t="n"/>
@@ -633,11 +633,11 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>没有编写小车接触晶石后重新生成晶石的代码</t>
+          <t>最后没有调用第六段</t>
         </is>
       </c>
       <c r="D6" s="2" t="n"/>
@@ -671,11 +671,11 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>将能量加40写成了设为40</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D7" s="2" t="n"/>
@@ -709,11 +709,11 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>多写了让晶石能量设为0的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D8" s="2" t="n"/>
@@ -751,7 +751,7 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>完全没写代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D9" s="2" t="n"/>
@@ -785,11 +785,11 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D10" s="2" t="n"/>
@@ -823,11 +823,11 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>将晶石能量加40写成了倒计时加40</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D11" s="2" t="n"/>
@@ -861,11 +861,11 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>未编写在判断语句中晶石能量增加和生成晶石的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D12" s="2" t="n"/>
@@ -899,11 +899,11 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D13" s="2" t="n"/>
@@ -937,11 +937,11 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>将晶石能量加40写成了加1</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D14" s="2" t="n"/>
@@ -975,11 +975,11 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D15" s="2" t="n"/>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D16" s="2" t="n"/>
@@ -1051,11 +1051,11 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D17" s="2" t="n"/>
@@ -1089,11 +1089,11 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D18" s="2" t="n"/>
@@ -1127,11 +1127,11 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D19" s="2" t="n"/>
@@ -1165,11 +1165,11 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>循环中没有调用生成晶石的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D20" s="2" t="n"/>
@@ -1203,11 +1203,11 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D21" s="2" t="n"/>
@@ -1241,11 +1241,11 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环次数错误</t>
         </is>
       </c>
       <c r="D22" s="2" t="n"/>
@@ -1279,11 +1279,11 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>将晶石能量加40写成了加5</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D23" s="2" t="n"/>
@@ -1317,11 +1317,11 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>完全没写代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D24" s="2" t="n"/>
@@ -1355,11 +1355,11 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>循环中没有调用生成晶石的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D25" s="2" t="n"/>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D26" s="2" t="n"/>
@@ -1431,11 +1431,11 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D27" s="2" t="n"/>
@@ -1469,11 +1469,11 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>完全没写代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D28" s="2" t="n"/>
@@ -1507,11 +1507,11 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D29" s="2" t="n"/>
@@ -1545,11 +1545,11 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>将能量加40写成了设为40</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D30" s="2" t="n"/>
@@ -1583,11 +1583,11 @@
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D31" s="2" t="n"/>
@@ -1621,11 +1621,11 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>没有编写循环函数</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D32" s="2" t="n"/>
@@ -1659,11 +1659,11 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D33" s="2" t="n"/>
@@ -1697,11 +1697,11 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环内缺少内容</t>
         </is>
       </c>
       <c r="D34" s="2" t="n"/>
@@ -1735,11 +1735,11 @@
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>没有使用循环</t>
         </is>
       </c>
       <c r="D35" s="2" t="n"/>
@@ -1773,11 +1773,11 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D36" s="2" t="n"/>
@@ -1811,11 +1811,11 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>将探险车错误写为小探险车</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D37" s="2" t="n"/>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D38" s="2" t="n"/>
@@ -1887,11 +1887,11 @@
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D39" s="2" t="n"/>
@@ -1925,11 +1925,11 @@
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>将能量加40写成了设为40</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D40" s="2" t="n"/>
@@ -1963,11 +1963,11 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>生成晶石代码书写后结构被破坏</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D41" s="2" t="n"/>
@@ -1997,15 +1997,15 @@
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>pad</t>
+          <t>电脑</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D42" s="2" t="n"/>
@@ -2039,11 +2039,11 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D43" s="2" t="n"/>
@@ -2077,11 +2077,11 @@
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D44" s="2" t="n"/>
@@ -2115,11 +2115,11 @@
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>完全没写生成晶石的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D45" s="2" t="n"/>
@@ -2153,11 +2153,11 @@
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D46" s="2" t="n"/>
@@ -2191,11 +2191,11 @@
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>循环中没有调用生成晶石的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D47" s="2" t="n"/>
@@ -2229,11 +2229,11 @@
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>生成晶石代码中没有使用随机数</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D48" s="2" t="n"/>
@@ -2267,11 +2267,11 @@
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>循环中没有调用生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D49" s="2" t="n"/>
@@ -2305,11 +2305,11 @@
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>完全没写生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D50" s="2" t="n"/>
@@ -2343,11 +2343,11 @@
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>循环中和启动时没有调用生成晶石的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D51" s="2" t="n"/>
@@ -2377,15 +2377,15 @@
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>pad</t>
+          <t>电脑</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>完全没写生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D52" s="2" t="n"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D53" s="2" t="n"/>
@@ -2457,11 +2457,11 @@
         </is>
       </c>
       <c r="B54" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D54" s="2" t="n"/>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D55" s="2" t="n"/>
@@ -2533,11 +2533,11 @@
         </is>
       </c>
       <c r="B56" s="2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D56" s="2" t="n"/>
@@ -2571,11 +2571,11 @@
         </is>
       </c>
       <c r="B57" s="2" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>将晶石y-探险车y写成晶石y-晶石x</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D57" s="2" t="n"/>
@@ -2609,11 +2609,11 @@
         </is>
       </c>
       <c r="B58" s="2" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>将晶石y-探险车y写成晶石y-晶石x</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D58" s="2" t="n"/>
@@ -2647,11 +2647,11 @@
         </is>
       </c>
       <c r="B59" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D59" s="2" t="n"/>
@@ -2685,11 +2685,11 @@
         </is>
       </c>
       <c r="B60" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D60" s="2" t="n"/>
@@ -2723,11 +2723,11 @@
         </is>
       </c>
       <c r="B61" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D61" s="2" t="n"/>
@@ -2761,11 +2761,11 @@
         </is>
       </c>
       <c r="B62" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D62" s="2" t="n"/>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D63" s="2" t="n"/>
@@ -2837,11 +2837,11 @@
         </is>
       </c>
       <c r="B64" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D64" s="2" t="n"/>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D65" s="2" t="n"/>
@@ -2913,11 +2913,11 @@
         </is>
       </c>
       <c r="B66" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D66" s="2" t="n"/>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D67" s="2" t="n"/>
@@ -2985,15 +2985,15 @@
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>电脑</t>
+          <t>pad</t>
         </is>
       </c>
       <c r="B68" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D68" s="2" t="n"/>
@@ -3027,11 +3027,11 @@
         </is>
       </c>
       <c r="B69" s="2" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>没有编写小车碰见晶石的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D69" s="2" t="n"/>
@@ -3065,11 +3065,11 @@
         </is>
       </c>
       <c r="B70" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D70" s="2" t="n"/>
@@ -3103,11 +3103,11 @@
         </is>
       </c>
       <c r="B71" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D71" s="2" t="n"/>
@@ -3141,11 +3141,11 @@
         </is>
       </c>
       <c r="B72" s="2" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>将晶石能量加40写成了加1</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D72" s="2" t="n"/>
@@ -3179,11 +3179,11 @@
         </is>
       </c>
       <c r="B73" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>循环次序错误</t>
         </is>
       </c>
       <c r="D73" s="2" t="n"/>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D74" s="2" t="n"/>
@@ -3255,11 +3255,11 @@
         </is>
       </c>
       <c r="B75" s="2" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>将坐标相剪写为大于判断语句</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D75" s="2" t="n"/>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>完全没写代码</t>
+          <t>错写在音符角色中</t>
         </is>
       </c>
       <c r="D76" s="2" t="n"/>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>将生成晶石的代码错误放在了判断语句外</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D77" s="2" t="n"/>
@@ -3369,11 +3369,11 @@
         </is>
       </c>
       <c r="B78" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>完全没写代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D78" s="2" t="n"/>
@@ -3407,11 +3407,11 @@
         </is>
       </c>
       <c r="B79" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>循环内缺少内容</t>
         </is>
       </c>
       <c r="D79" s="2" t="n"/>
@@ -3445,11 +3445,11 @@
         </is>
       </c>
       <c r="B80" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D80" s="2" t="n"/>
@@ -3483,11 +3483,11 @@
         </is>
       </c>
       <c r="B81" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>没有编写让晶石随着小车相对移动的代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D81" s="2" t="n"/>
@@ -3521,11 +3521,11 @@
         </is>
       </c>
       <c r="B82" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>完全没写代码</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D82" s="2" t="n"/>
@@ -3559,11 +3559,11 @@
         </is>
       </c>
       <c r="B83" s="2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>没有编写循环函数</t>
+          <t>完全没写</t>
         </is>
       </c>
       <c r="D83" s="2" t="n"/>
@@ -3597,11 +3597,11 @@
         </is>
       </c>
       <c r="B84" s="2" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>启动时没有调用生成晶石的代码</t>
+          <t>循环内缺少内容</t>
         </is>
       </c>
       <c r="D84" s="2" t="n"/>
@@ -3628,6 +3628,994 @@
       <c r="Y84" s="2" t="n"/>
       <c r="Z84" s="2" t="n"/>
     </row>
+    <row r="85">
+      <c r="A85" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="n"/>
+      <c r="E85" s="2" t="n"/>
+      <c r="F85" s="2" t="n"/>
+      <c r="G85" s="2" t="n"/>
+      <c r="H85" s="2" t="n"/>
+      <c r="I85" s="2" t="n"/>
+      <c r="J85" s="2" t="n"/>
+      <c r="K85" s="2" t="n"/>
+      <c r="L85" s="2" t="n"/>
+      <c r="M85" s="2" t="n"/>
+      <c r="N85" s="2" t="n"/>
+      <c r="O85" s="2" t="n"/>
+      <c r="P85" s="2" t="n"/>
+      <c r="Q85" s="2" t="n"/>
+      <c r="R85" s="2" t="n"/>
+      <c r="S85" s="2" t="n"/>
+      <c r="T85" s="2" t="n"/>
+      <c r="U85" s="2" t="n"/>
+      <c r="V85" s="2" t="n"/>
+      <c r="W85" s="2" t="n"/>
+      <c r="X85" s="2" t="n"/>
+      <c r="Y85" s="2" t="n"/>
+      <c r="Z85" s="2" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="n"/>
+      <c r="E86" s="2" t="n"/>
+      <c r="F86" s="2" t="n"/>
+      <c r="G86" s="2" t="n"/>
+      <c r="H86" s="2" t="n"/>
+      <c r="I86" s="2" t="n"/>
+      <c r="J86" s="2" t="n"/>
+      <c r="K86" s="2" t="n"/>
+      <c r="L86" s="2" t="n"/>
+      <c r="M86" s="2" t="n"/>
+      <c r="N86" s="2" t="n"/>
+      <c r="O86" s="2" t="n"/>
+      <c r="P86" s="2" t="n"/>
+      <c r="Q86" s="2" t="n"/>
+      <c r="R86" s="2" t="n"/>
+      <c r="S86" s="2" t="n"/>
+      <c r="T86" s="2" t="n"/>
+      <c r="U86" s="2" t="n"/>
+      <c r="V86" s="2" t="n"/>
+      <c r="W86" s="2" t="n"/>
+      <c r="X86" s="2" t="n"/>
+      <c r="Y86" s="2" t="n"/>
+      <c r="Z86" s="2" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="n"/>
+      <c r="E87" s="2" t="n"/>
+      <c r="F87" s="2" t="n"/>
+      <c r="G87" s="2" t="n"/>
+      <c r="H87" s="2" t="n"/>
+      <c r="I87" s="2" t="n"/>
+      <c r="J87" s="2" t="n"/>
+      <c r="K87" s="2" t="n"/>
+      <c r="L87" s="2" t="n"/>
+      <c r="M87" s="2" t="n"/>
+      <c r="N87" s="2" t="n"/>
+      <c r="O87" s="2" t="n"/>
+      <c r="P87" s="2" t="n"/>
+      <c r="Q87" s="2" t="n"/>
+      <c r="R87" s="2" t="n"/>
+      <c r="S87" s="2" t="n"/>
+      <c r="T87" s="2" t="n"/>
+      <c r="U87" s="2" t="n"/>
+      <c r="V87" s="2" t="n"/>
+      <c r="W87" s="2" t="n"/>
+      <c r="X87" s="2" t="n"/>
+      <c r="Y87" s="2" t="n"/>
+      <c r="Z87" s="2" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>多写了等待语句</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="n"/>
+      <c r="E88" s="2" t="n"/>
+      <c r="F88" s="2" t="n"/>
+      <c r="G88" s="2" t="n"/>
+      <c r="H88" s="2" t="n"/>
+      <c r="I88" s="2" t="n"/>
+      <c r="J88" s="2" t="n"/>
+      <c r="K88" s="2" t="n"/>
+      <c r="L88" s="2" t="n"/>
+      <c r="M88" s="2" t="n"/>
+      <c r="N88" s="2" t="n"/>
+      <c r="O88" s="2" t="n"/>
+      <c r="P88" s="2" t="n"/>
+      <c r="Q88" s="2" t="n"/>
+      <c r="R88" s="2" t="n"/>
+      <c r="S88" s="2" t="n"/>
+      <c r="T88" s="2" t="n"/>
+      <c r="U88" s="2" t="n"/>
+      <c r="V88" s="2" t="n"/>
+      <c r="W88" s="2" t="n"/>
+      <c r="X88" s="2" t="n"/>
+      <c r="Y88" s="2" t="n"/>
+      <c r="Z88" s="2" t="n"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C89" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="n"/>
+      <c r="E89" s="2" t="n"/>
+      <c r="F89" s="2" t="n"/>
+      <c r="G89" s="2" t="n"/>
+      <c r="H89" s="2" t="n"/>
+      <c r="I89" s="2" t="n"/>
+      <c r="J89" s="2" t="n"/>
+      <c r="K89" s="2" t="n"/>
+      <c r="L89" s="2" t="n"/>
+      <c r="M89" s="2" t="n"/>
+      <c r="N89" s="2" t="n"/>
+      <c r="O89" s="2" t="n"/>
+      <c r="P89" s="2" t="n"/>
+      <c r="Q89" s="2" t="n"/>
+      <c r="R89" s="2" t="n"/>
+      <c r="S89" s="2" t="n"/>
+      <c r="T89" s="2" t="n"/>
+      <c r="U89" s="2" t="n"/>
+      <c r="V89" s="2" t="n"/>
+      <c r="W89" s="2" t="n"/>
+      <c r="X89" s="2" t="n"/>
+      <c r="Y89" s="2" t="n"/>
+      <c r="Z89" s="2" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>最后没有调用第六段</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="n"/>
+      <c r="E90" s="2" t="n"/>
+      <c r="F90" s="2" t="n"/>
+      <c r="G90" s="2" t="n"/>
+      <c r="H90" s="2" t="n"/>
+      <c r="I90" s="2" t="n"/>
+      <c r="J90" s="2" t="n"/>
+      <c r="K90" s="2" t="n"/>
+      <c r="L90" s="2" t="n"/>
+      <c r="M90" s="2" t="n"/>
+      <c r="N90" s="2" t="n"/>
+      <c r="O90" s="2" t="n"/>
+      <c r="P90" s="2" t="n"/>
+      <c r="Q90" s="2" t="n"/>
+      <c r="R90" s="2" t="n"/>
+      <c r="S90" s="2" t="n"/>
+      <c r="T90" s="2" t="n"/>
+      <c r="U90" s="2" t="n"/>
+      <c r="V90" s="2" t="n"/>
+      <c r="W90" s="2" t="n"/>
+      <c r="X90" s="2" t="n"/>
+      <c r="Y90" s="2" t="n"/>
+      <c r="Z90" s="2" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" s="2" t="inlineStr">
+        <is>
+          <t>循环次序错误</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="n"/>
+      <c r="E91" s="2" t="n"/>
+      <c r="F91" s="2" t="n"/>
+      <c r="G91" s="2" t="n"/>
+      <c r="H91" s="2" t="n"/>
+      <c r="I91" s="2" t="n"/>
+      <c r="J91" s="2" t="n"/>
+      <c r="K91" s="2" t="n"/>
+      <c r="L91" s="2" t="n"/>
+      <c r="M91" s="2" t="n"/>
+      <c r="N91" s="2" t="n"/>
+      <c r="O91" s="2" t="n"/>
+      <c r="P91" s="2" t="n"/>
+      <c r="Q91" s="2" t="n"/>
+      <c r="R91" s="2" t="n"/>
+      <c r="S91" s="2" t="n"/>
+      <c r="T91" s="2" t="n"/>
+      <c r="U91" s="2" t="n"/>
+      <c r="V91" s="2" t="n"/>
+      <c r="W91" s="2" t="n"/>
+      <c r="X91" s="2" t="n"/>
+      <c r="Y91" s="2" t="n"/>
+      <c r="Z91" s="2" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="n"/>
+      <c r="E92" s="2" t="n"/>
+      <c r="F92" s="2" t="n"/>
+      <c r="G92" s="2" t="n"/>
+      <c r="H92" s="2" t="n"/>
+      <c r="I92" s="2" t="n"/>
+      <c r="J92" s="2" t="n"/>
+      <c r="K92" s="2" t="n"/>
+      <c r="L92" s="2" t="n"/>
+      <c r="M92" s="2" t="n"/>
+      <c r="N92" s="2" t="n"/>
+      <c r="O92" s="2" t="n"/>
+      <c r="P92" s="2" t="n"/>
+      <c r="Q92" s="2" t="n"/>
+      <c r="R92" s="2" t="n"/>
+      <c r="S92" s="2" t="n"/>
+      <c r="T92" s="2" t="n"/>
+      <c r="U92" s="2" t="n"/>
+      <c r="V92" s="2" t="n"/>
+      <c r="W92" s="2" t="n"/>
+      <c r="X92" s="2" t="n"/>
+      <c r="Y92" s="2" t="n"/>
+      <c r="Z92" s="2" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B93" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C93" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="n"/>
+      <c r="E93" s="2" t="n"/>
+      <c r="F93" s="2" t="n"/>
+      <c r="G93" s="2" t="n"/>
+      <c r="H93" s="2" t="n"/>
+      <c r="I93" s="2" t="n"/>
+      <c r="J93" s="2" t="n"/>
+      <c r="K93" s="2" t="n"/>
+      <c r="L93" s="2" t="n"/>
+      <c r="M93" s="2" t="n"/>
+      <c r="N93" s="2" t="n"/>
+      <c r="O93" s="2" t="n"/>
+      <c r="P93" s="2" t="n"/>
+      <c r="Q93" s="2" t="n"/>
+      <c r="R93" s="2" t="n"/>
+      <c r="S93" s="2" t="n"/>
+      <c r="T93" s="2" t="n"/>
+      <c r="U93" s="2" t="n"/>
+      <c r="V93" s="2" t="n"/>
+      <c r="W93" s="2" t="n"/>
+      <c r="X93" s="2" t="n"/>
+      <c r="Y93" s="2" t="n"/>
+      <c r="Z93" s="2" t="n"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>循环次序错误</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="n"/>
+      <c r="E94" s="2" t="n"/>
+      <c r="F94" s="2" t="n"/>
+      <c r="G94" s="2" t="n"/>
+      <c r="H94" s="2" t="n"/>
+      <c r="I94" s="2" t="n"/>
+      <c r="J94" s="2" t="n"/>
+      <c r="K94" s="2" t="n"/>
+      <c r="L94" s="2" t="n"/>
+      <c r="M94" s="2" t="n"/>
+      <c r="N94" s="2" t="n"/>
+      <c r="O94" s="2" t="n"/>
+      <c r="P94" s="2" t="n"/>
+      <c r="Q94" s="2" t="n"/>
+      <c r="R94" s="2" t="n"/>
+      <c r="S94" s="2" t="n"/>
+      <c r="T94" s="2" t="n"/>
+      <c r="U94" s="2" t="n"/>
+      <c r="V94" s="2" t="n"/>
+      <c r="W94" s="2" t="n"/>
+      <c r="X94" s="2" t="n"/>
+      <c r="Y94" s="2" t="n"/>
+      <c r="Z94" s="2" t="n"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="n"/>
+      <c r="E95" s="2" t="n"/>
+      <c r="F95" s="2" t="n"/>
+      <c r="G95" s="2" t="n"/>
+      <c r="H95" s="2" t="n"/>
+      <c r="I95" s="2" t="n"/>
+      <c r="J95" s="2" t="n"/>
+      <c r="K95" s="2" t="n"/>
+      <c r="L95" s="2" t="n"/>
+      <c r="M95" s="2" t="n"/>
+      <c r="N95" s="2" t="n"/>
+      <c r="O95" s="2" t="n"/>
+      <c r="P95" s="2" t="n"/>
+      <c r="Q95" s="2" t="n"/>
+      <c r="R95" s="2" t="n"/>
+      <c r="S95" s="2" t="n"/>
+      <c r="T95" s="2" t="n"/>
+      <c r="U95" s="2" t="n"/>
+      <c r="V95" s="2" t="n"/>
+      <c r="W95" s="2" t="n"/>
+      <c r="X95" s="2" t="n"/>
+      <c r="Y95" s="2" t="n"/>
+      <c r="Z95" s="2" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="n"/>
+      <c r="E96" s="2" t="n"/>
+      <c r="F96" s="2" t="n"/>
+      <c r="G96" s="2" t="n"/>
+      <c r="H96" s="2" t="n"/>
+      <c r="I96" s="2" t="n"/>
+      <c r="J96" s="2" t="n"/>
+      <c r="K96" s="2" t="n"/>
+      <c r="L96" s="2" t="n"/>
+      <c r="M96" s="2" t="n"/>
+      <c r="N96" s="2" t="n"/>
+      <c r="O96" s="2" t="n"/>
+      <c r="P96" s="2" t="n"/>
+      <c r="Q96" s="2" t="n"/>
+      <c r="R96" s="2" t="n"/>
+      <c r="S96" s="2" t="n"/>
+      <c r="T96" s="2" t="n"/>
+      <c r="U96" s="2" t="n"/>
+      <c r="V96" s="2" t="n"/>
+      <c r="W96" s="2" t="n"/>
+      <c r="X96" s="2" t="n"/>
+      <c r="Y96" s="2" t="n"/>
+      <c r="Z96" s="2" t="n"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="n"/>
+      <c r="E97" s="2" t="n"/>
+      <c r="F97" s="2" t="n"/>
+      <c r="G97" s="2" t="n"/>
+      <c r="H97" s="2" t="n"/>
+      <c r="I97" s="2" t="n"/>
+      <c r="J97" s="2" t="n"/>
+      <c r="K97" s="2" t="n"/>
+      <c r="L97" s="2" t="n"/>
+      <c r="M97" s="2" t="n"/>
+      <c r="N97" s="2" t="n"/>
+      <c r="O97" s="2" t="n"/>
+      <c r="P97" s="2" t="n"/>
+      <c r="Q97" s="2" t="n"/>
+      <c r="R97" s="2" t="n"/>
+      <c r="S97" s="2" t="n"/>
+      <c r="T97" s="2" t="n"/>
+      <c r="U97" s="2" t="n"/>
+      <c r="V97" s="2" t="n"/>
+      <c r="W97" s="2" t="n"/>
+      <c r="X97" s="2" t="n"/>
+      <c r="Y97" s="2" t="n"/>
+      <c r="Z97" s="2" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>循环次序错误</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="n"/>
+      <c r="E98" s="2" t="n"/>
+      <c r="F98" s="2" t="n"/>
+      <c r="G98" s="2" t="n"/>
+      <c r="H98" s="2" t="n"/>
+      <c r="I98" s="2" t="n"/>
+      <c r="J98" s="2" t="n"/>
+      <c r="K98" s="2" t="n"/>
+      <c r="L98" s="2" t="n"/>
+      <c r="M98" s="2" t="n"/>
+      <c r="N98" s="2" t="n"/>
+      <c r="O98" s="2" t="n"/>
+      <c r="P98" s="2" t="n"/>
+      <c r="Q98" s="2" t="n"/>
+      <c r="R98" s="2" t="n"/>
+      <c r="S98" s="2" t="n"/>
+      <c r="T98" s="2" t="n"/>
+      <c r="U98" s="2" t="n"/>
+      <c r="V98" s="2" t="n"/>
+      <c r="W98" s="2" t="n"/>
+      <c r="X98" s="2" t="n"/>
+      <c r="Y98" s="2" t="n"/>
+      <c r="Z98" s="2" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B99" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="n"/>
+      <c r="E99" s="2" t="n"/>
+      <c r="F99" s="2" t="n"/>
+      <c r="G99" s="2" t="n"/>
+      <c r="H99" s="2" t="n"/>
+      <c r="I99" s="2" t="n"/>
+      <c r="J99" s="2" t="n"/>
+      <c r="K99" s="2" t="n"/>
+      <c r="L99" s="2" t="n"/>
+      <c r="M99" s="2" t="n"/>
+      <c r="N99" s="2" t="n"/>
+      <c r="O99" s="2" t="n"/>
+      <c r="P99" s="2" t="n"/>
+      <c r="Q99" s="2" t="n"/>
+      <c r="R99" s="2" t="n"/>
+      <c r="S99" s="2" t="n"/>
+      <c r="T99" s="2" t="n"/>
+      <c r="U99" s="2" t="n"/>
+      <c r="V99" s="2" t="n"/>
+      <c r="W99" s="2" t="n"/>
+      <c r="X99" s="2" t="n"/>
+      <c r="Y99" s="2" t="n"/>
+      <c r="Z99" s="2" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>最后没有调用第六段</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="n"/>
+      <c r="E100" s="2" t="n"/>
+      <c r="F100" s="2" t="n"/>
+      <c r="G100" s="2" t="n"/>
+      <c r="H100" s="2" t="n"/>
+      <c r="I100" s="2" t="n"/>
+      <c r="J100" s="2" t="n"/>
+      <c r="K100" s="2" t="n"/>
+      <c r="L100" s="2" t="n"/>
+      <c r="M100" s="2" t="n"/>
+      <c r="N100" s="2" t="n"/>
+      <c r="O100" s="2" t="n"/>
+      <c r="P100" s="2" t="n"/>
+      <c r="Q100" s="2" t="n"/>
+      <c r="R100" s="2" t="n"/>
+      <c r="S100" s="2" t="n"/>
+      <c r="T100" s="2" t="n"/>
+      <c r="U100" s="2" t="n"/>
+      <c r="V100" s="2" t="n"/>
+      <c r="W100" s="2" t="n"/>
+      <c r="X100" s="2" t="n"/>
+      <c r="Y100" s="2" t="n"/>
+      <c r="Z100" s="2" t="n"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="n"/>
+      <c r="E101" s="2" t="n"/>
+      <c r="F101" s="2" t="n"/>
+      <c r="G101" s="2" t="n"/>
+      <c r="H101" s="2" t="n"/>
+      <c r="I101" s="2" t="n"/>
+      <c r="J101" s="2" t="n"/>
+      <c r="K101" s="2" t="n"/>
+      <c r="L101" s="2" t="n"/>
+      <c r="M101" s="2" t="n"/>
+      <c r="N101" s="2" t="n"/>
+      <c r="O101" s="2" t="n"/>
+      <c r="P101" s="2" t="n"/>
+      <c r="Q101" s="2" t="n"/>
+      <c r="R101" s="2" t="n"/>
+      <c r="S101" s="2" t="n"/>
+      <c r="T101" s="2" t="n"/>
+      <c r="U101" s="2" t="n"/>
+      <c r="V101" s="2" t="n"/>
+      <c r="W101" s="2" t="n"/>
+      <c r="X101" s="2" t="n"/>
+      <c r="Y101" s="2" t="n"/>
+      <c r="Z101" s="2" t="n"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>没有使用循环</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="n"/>
+      <c r="E102" s="2" t="n"/>
+      <c r="F102" s="2" t="n"/>
+      <c r="G102" s="2" t="n"/>
+      <c r="H102" s="2" t="n"/>
+      <c r="I102" s="2" t="n"/>
+      <c r="J102" s="2" t="n"/>
+      <c r="K102" s="2" t="n"/>
+      <c r="L102" s="2" t="n"/>
+      <c r="M102" s="2" t="n"/>
+      <c r="N102" s="2" t="n"/>
+      <c r="O102" s="2" t="n"/>
+      <c r="P102" s="2" t="n"/>
+      <c r="Q102" s="2" t="n"/>
+      <c r="R102" s="2" t="n"/>
+      <c r="S102" s="2" t="n"/>
+      <c r="T102" s="2" t="n"/>
+      <c r="U102" s="2" t="n"/>
+      <c r="V102" s="2" t="n"/>
+      <c r="W102" s="2" t="n"/>
+      <c r="X102" s="2" t="n"/>
+      <c r="Y102" s="2" t="n"/>
+      <c r="Z102" s="2" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B103" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C103" s="2" t="inlineStr">
+        <is>
+          <t>循环次序错误</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="n"/>
+      <c r="E103" s="2" t="n"/>
+      <c r="F103" s="2" t="n"/>
+      <c r="G103" s="2" t="n"/>
+      <c r="H103" s="2" t="n"/>
+      <c r="I103" s="2" t="n"/>
+      <c r="J103" s="2" t="n"/>
+      <c r="K103" s="2" t="n"/>
+      <c r="L103" s="2" t="n"/>
+      <c r="M103" s="2" t="n"/>
+      <c r="N103" s="2" t="n"/>
+      <c r="O103" s="2" t="n"/>
+      <c r="P103" s="2" t="n"/>
+      <c r="Q103" s="2" t="n"/>
+      <c r="R103" s="2" t="n"/>
+      <c r="S103" s="2" t="n"/>
+      <c r="T103" s="2" t="n"/>
+      <c r="U103" s="2" t="n"/>
+      <c r="V103" s="2" t="n"/>
+      <c r="W103" s="2" t="n"/>
+      <c r="X103" s="2" t="n"/>
+      <c r="Y103" s="2" t="n"/>
+      <c r="Z103" s="2" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="n"/>
+      <c r="E104" s="2" t="n"/>
+      <c r="F104" s="2" t="n"/>
+      <c r="G104" s="2" t="n"/>
+      <c r="H104" s="2" t="n"/>
+      <c r="I104" s="2" t="n"/>
+      <c r="J104" s="2" t="n"/>
+      <c r="K104" s="2" t="n"/>
+      <c r="L104" s="2" t="n"/>
+      <c r="M104" s="2" t="n"/>
+      <c r="N104" s="2" t="n"/>
+      <c r="O104" s="2" t="n"/>
+      <c r="P104" s="2" t="n"/>
+      <c r="Q104" s="2" t="n"/>
+      <c r="R104" s="2" t="n"/>
+      <c r="S104" s="2" t="n"/>
+      <c r="T104" s="2" t="n"/>
+      <c r="U104" s="2" t="n"/>
+      <c r="V104" s="2" t="n"/>
+      <c r="W104" s="2" t="n"/>
+      <c r="X104" s="2" t="n"/>
+      <c r="Y104" s="2" t="n"/>
+      <c r="Z104" s="2" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B105" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C105" s="2" t="inlineStr">
+        <is>
+          <t>循环次序错误</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="n"/>
+      <c r="E105" s="2" t="n"/>
+      <c r="F105" s="2" t="n"/>
+      <c r="G105" s="2" t="n"/>
+      <c r="H105" s="2" t="n"/>
+      <c r="I105" s="2" t="n"/>
+      <c r="J105" s="2" t="n"/>
+      <c r="K105" s="2" t="n"/>
+      <c r="L105" s="2" t="n"/>
+      <c r="M105" s="2" t="n"/>
+      <c r="N105" s="2" t="n"/>
+      <c r="O105" s="2" t="n"/>
+      <c r="P105" s="2" t="n"/>
+      <c r="Q105" s="2" t="n"/>
+      <c r="R105" s="2" t="n"/>
+      <c r="S105" s="2" t="n"/>
+      <c r="T105" s="2" t="n"/>
+      <c r="U105" s="2" t="n"/>
+      <c r="V105" s="2" t="n"/>
+      <c r="W105" s="2" t="n"/>
+      <c r="X105" s="2" t="n"/>
+      <c r="Y105" s="2" t="n"/>
+      <c r="Z105" s="2" t="n"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B106" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>循环次序错误</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="n"/>
+      <c r="E106" s="2" t="n"/>
+      <c r="F106" s="2" t="n"/>
+      <c r="G106" s="2" t="n"/>
+      <c r="H106" s="2" t="n"/>
+      <c r="I106" s="2" t="n"/>
+      <c r="J106" s="2" t="n"/>
+      <c r="K106" s="2" t="n"/>
+      <c r="L106" s="2" t="n"/>
+      <c r="M106" s="2" t="n"/>
+      <c r="N106" s="2" t="n"/>
+      <c r="O106" s="2" t="n"/>
+      <c r="P106" s="2" t="n"/>
+      <c r="Q106" s="2" t="n"/>
+      <c r="R106" s="2" t="n"/>
+      <c r="S106" s="2" t="n"/>
+      <c r="T106" s="2" t="n"/>
+      <c r="U106" s="2" t="n"/>
+      <c r="V106" s="2" t="n"/>
+      <c r="W106" s="2" t="n"/>
+      <c r="X106" s="2" t="n"/>
+      <c r="Y106" s="2" t="n"/>
+      <c r="Z106" s="2" t="n"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B107" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C107" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D107" s="2" t="n"/>
+      <c r="E107" s="2" t="n"/>
+      <c r="F107" s="2" t="n"/>
+      <c r="G107" s="2" t="n"/>
+      <c r="H107" s="2" t="n"/>
+      <c r="I107" s="2" t="n"/>
+      <c r="J107" s="2" t="n"/>
+      <c r="K107" s="2" t="n"/>
+      <c r="L107" s="2" t="n"/>
+      <c r="M107" s="2" t="n"/>
+      <c r="N107" s="2" t="n"/>
+      <c r="O107" s="2" t="n"/>
+      <c r="P107" s="2" t="n"/>
+      <c r="Q107" s="2" t="n"/>
+      <c r="R107" s="2" t="n"/>
+      <c r="S107" s="2" t="n"/>
+      <c r="T107" s="2" t="n"/>
+      <c r="U107" s="2" t="n"/>
+      <c r="V107" s="2" t="n"/>
+      <c r="W107" s="2" t="n"/>
+      <c r="X107" s="2" t="n"/>
+      <c r="Y107" s="2" t="n"/>
+      <c r="Z107" s="2" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B108" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="n"/>
+      <c r="E108" s="2" t="n"/>
+      <c r="F108" s="2" t="n"/>
+      <c r="G108" s="2" t="n"/>
+      <c r="H108" s="2" t="n"/>
+      <c r="I108" s="2" t="n"/>
+      <c r="J108" s="2" t="n"/>
+      <c r="K108" s="2" t="n"/>
+      <c r="L108" s="2" t="n"/>
+      <c r="M108" s="2" t="n"/>
+      <c r="N108" s="2" t="n"/>
+      <c r="O108" s="2" t="n"/>
+      <c r="P108" s="2" t="n"/>
+      <c r="Q108" s="2" t="n"/>
+      <c r="R108" s="2" t="n"/>
+      <c r="S108" s="2" t="n"/>
+      <c r="T108" s="2" t="n"/>
+      <c r="U108" s="2" t="n"/>
+      <c r="V108" s="2" t="n"/>
+      <c r="W108" s="2" t="n"/>
+      <c r="X108" s="2" t="n"/>
+      <c r="Y108" s="2" t="n"/>
+      <c r="Z108" s="2" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B109" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C109" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D109" s="2" t="n"/>
+      <c r="E109" s="2" t="n"/>
+      <c r="F109" s="2" t="n"/>
+      <c r="G109" s="2" t="n"/>
+      <c r="H109" s="2" t="n"/>
+      <c r="I109" s="2" t="n"/>
+      <c r="J109" s="2" t="n"/>
+      <c r="K109" s="2" t="n"/>
+      <c r="L109" s="2" t="n"/>
+      <c r="M109" s="2" t="n"/>
+      <c r="N109" s="2" t="n"/>
+      <c r="O109" s="2" t="n"/>
+      <c r="P109" s="2" t="n"/>
+      <c r="Q109" s="2" t="n"/>
+      <c r="R109" s="2" t="n"/>
+      <c r="S109" s="2" t="n"/>
+      <c r="T109" s="2" t="n"/>
+      <c r="U109" s="2" t="n"/>
+      <c r="V109" s="2" t="n"/>
+      <c r="W109" s="2" t="n"/>
+      <c r="X109" s="2" t="n"/>
+      <c r="Y109" s="2" t="n"/>
+      <c r="Z109" s="2" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>电脑</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C110" s="2" t="inlineStr">
+        <is>
+          <t>完全没写</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="n"/>
+      <c r="E110" s="2" t="n"/>
+      <c r="F110" s="2" t="n"/>
+      <c r="G110" s="2" t="n"/>
+      <c r="H110" s="2" t="n"/>
+      <c r="I110" s="2" t="n"/>
+      <c r="J110" s="2" t="n"/>
+      <c r="K110" s="2" t="n"/>
+      <c r="L110" s="2" t="n"/>
+      <c r="M110" s="2" t="n"/>
+      <c r="N110" s="2" t="n"/>
+      <c r="O110" s="2" t="n"/>
+      <c r="P110" s="2" t="n"/>
+      <c r="Q110" s="2" t="n"/>
+      <c r="R110" s="2" t="n"/>
+      <c r="S110" s="2" t="n"/>
+      <c r="T110" s="2" t="n"/>
+      <c r="U110" s="2" t="n"/>
+      <c r="V110" s="2" t="n"/>
+      <c r="W110" s="2" t="n"/>
+      <c r="X110" s="2" t="n"/>
+      <c r="Y110" s="2" t="n"/>
+      <c r="Z110" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>